<commit_message>
full AUC with empys fix, mismatch y_col and column
</commit_message>
<xml_diff>
--- a/test_result/multiindex_saving.xlsx
+++ b/test_result/multiindex_saving.xlsx
@@ -433,22 +433,22 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>4</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -456,22 +456,22 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -479,22 +479,22 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -502,13 +502,13 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>4</v>

</xml_diff>